<commit_message>
updated processing FIN001-report.ipynb scripts 10/29/25
</commit_message>
<xml_diff>
--- a/Input_Files/BiWeekly Paycheck Dates.xlsx
+++ b/Input_Files/BiWeekly Paycheck Dates.xlsx
@@ -5,16 +5,19 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ldoyle\Box\LDoyle\DELETE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\awidjaja\Documents\RFL- POC\Input_Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E7FF3735-BFD5-44DB-B30A-4A955A2D7A3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AAFB40E-0A26-4EB1-BEBD-C80983E6D895}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{62EA33E2-6161-4099-BDF8-3AE4BBC65D99}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{62EA33E2-6161-4099-BDF8-3AE4BBC65D99}"/>
   </bookViews>
   <sheets>
     <sheet name="Bi-Weekly Paycheck Dates" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Bi-Weekly Paycheck Dates'!$A$1:$A$147</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -57,18 +60,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.749992370372631"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -83,15 +80,39 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFA6C9EC"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFA6C9EC"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFA6C9EC"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -421,19 +442,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C55E9EE7-05DB-43E6-A4E4-0C41AA9632D9}">
-  <dimension ref="A1:B160"/>
+  <dimension ref="A1:D147"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -441,7 +462,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43838</v>
       </c>
@@ -449,7 +470,7 @@
         <v>43838</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43852</v>
       </c>
@@ -457,7 +478,7 @@
         <v>43866</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>43866</v>
       </c>
@@ -465,7 +486,7 @@
         <v>43894</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>43880</v>
       </c>
@@ -473,7 +494,7 @@
         <v>43922</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>43894</v>
       </c>
@@ -481,7 +502,7 @@
         <v>43964</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>43908</v>
       </c>
@@ -489,7 +510,7 @@
         <v>43992</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>43922</v>
       </c>
@@ -497,7 +518,7 @@
         <v>44020</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>43936</v>
       </c>
@@ -505,957 +526,898 @@
         <v>44048</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="2">
-        <v>43950</v>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>43964</v>
       </c>
       <c r="B10" s="1">
         <v>44076</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>43964</v>
+        <v>43978</v>
       </c>
       <c r="B11" s="1">
         <v>44118</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>43978</v>
+        <v>43992</v>
       </c>
       <c r="B12" s="1">
         <v>44145</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>43992</v>
+        <v>44006</v>
       </c>
       <c r="B13" s="1">
         <v>44174</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>44006</v>
+        <v>44020</v>
       </c>
       <c r="B14" s="1">
         <v>44202</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>44020</v>
+        <v>44034</v>
       </c>
       <c r="B15" s="1">
         <v>44230</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>44034</v>
+        <v>44048</v>
       </c>
       <c r="B16" s="1">
         <v>44258</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>44048</v>
+        <v>44062</v>
       </c>
       <c r="B17" s="1">
         <v>44300</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>44062</v>
+        <v>44076</v>
       </c>
       <c r="B18" s="1">
         <v>44328</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>44076</v>
+        <v>44090</v>
       </c>
       <c r="B19" s="1">
         <v>44356</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>44090</v>
+        <v>44118</v>
       </c>
       <c r="B20" s="1">
         <v>44384</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="2">
-        <v>44104</v>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>44132</v>
       </c>
       <c r="B21" s="1">
         <v>44412</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>44118</v>
+        <v>44145</v>
       </c>
       <c r="B22" s="1">
         <v>44440</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>44132</v>
+        <v>44160</v>
       </c>
       <c r="B23" s="1">
         <v>44482</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>44145</v>
+        <v>44174</v>
       </c>
       <c r="B24" s="1">
         <v>44510</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>44160</v>
+        <v>44188</v>
       </c>
       <c r="B25" s="1">
         <v>44538</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>44174</v>
+        <v>44202</v>
       </c>
       <c r="B26" s="1">
         <v>44566</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>44188</v>
+        <v>44216</v>
       </c>
       <c r="B27" s="1">
         <v>44594</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>44202</v>
+        <v>44230</v>
       </c>
       <c r="B28" s="1">
         <v>44622</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>44216</v>
+        <v>44244</v>
       </c>
       <c r="B29" s="1">
         <v>44664</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>44230</v>
+        <v>44258</v>
       </c>
       <c r="B30" s="1">
         <v>44692</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>44244</v>
+        <v>44272</v>
       </c>
       <c r="B31" s="1">
         <v>44720</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>44258</v>
+        <v>44300</v>
       </c>
       <c r="B32" s="1">
         <v>44748</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>44272</v>
+        <v>44314</v>
       </c>
       <c r="B33" s="1">
         <v>44776</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" s="2">
-        <v>44286</v>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>44328</v>
       </c>
       <c r="B34" s="1">
         <v>44818</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>44300</v>
+        <v>44342</v>
       </c>
       <c r="B35" s="1">
         <v>44846</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <v>44314</v>
+        <v>44356</v>
       </c>
       <c r="B36" s="1">
         <v>44874</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
-        <v>44328</v>
+        <v>44370</v>
       </c>
       <c r="B37" s="1">
         <v>44902</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
-        <v>44342</v>
+        <v>44384</v>
       </c>
       <c r="B38" s="1">
         <v>44930</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
-        <v>44356</v>
+        <v>44398</v>
       </c>
       <c r="B39" s="1">
         <v>44958</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
-        <v>44370</v>
+        <v>44412</v>
       </c>
       <c r="B40" s="1">
         <v>44986</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
-        <v>44384</v>
+        <v>44426</v>
       </c>
       <c r="B41" s="1">
         <v>45028</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
-        <v>44398</v>
+        <v>44440</v>
       </c>
       <c r="B42" s="1">
         <v>45056</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
-        <v>44412</v>
+        <v>44454</v>
       </c>
       <c r="B43" s="1">
         <v>45084</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
-        <v>44426</v>
+        <v>44482</v>
       </c>
       <c r="B44" s="1">
         <v>45112</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
-        <v>44440</v>
+        <v>44496</v>
       </c>
       <c r="B45" s="1">
         <v>45140</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
-        <v>44454</v>
+        <v>44510</v>
       </c>
       <c r="B46" s="1">
         <v>45182</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A47" s="2">
-        <v>44468</v>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>44524</v>
       </c>
       <c r="B47" s="1">
         <v>45210</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
-        <v>44482</v>
+        <v>44538</v>
       </c>
       <c r="B48" s="1">
         <v>45238</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
-        <v>44496</v>
+        <v>44552</v>
       </c>
       <c r="B49" s="1">
         <v>45266</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
-        <v>44510</v>
+        <v>44566</v>
       </c>
       <c r="B50" s="1">
         <v>45294</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
-        <v>44524</v>
+        <v>44580</v>
       </c>
       <c r="B51" s="1">
         <v>45336</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
-        <v>44538</v>
+        <v>44594</v>
       </c>
       <c r="B52" s="1">
         <v>45364</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
-        <v>44552</v>
+        <v>44608</v>
       </c>
       <c r="B53" s="1">
         <v>45392</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
-        <v>44566</v>
+        <v>44622</v>
       </c>
       <c r="B54" s="1">
         <v>45420</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
-        <v>44580</v>
+        <v>44636</v>
       </c>
       <c r="B55" s="1">
         <v>45448</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
-        <v>44594</v>
+        <v>44664</v>
       </c>
       <c r="B56" s="1">
         <v>45476</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
-        <v>44608</v>
+        <v>44678</v>
       </c>
       <c r="B57" s="1">
         <v>45518</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
-        <v>44622</v>
+        <v>44692</v>
       </c>
       <c r="B58" s="1">
         <v>45546</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
-        <v>44636</v>
+        <v>44706</v>
       </c>
       <c r="B59" s="1">
         <v>45574</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A60" s="2">
-        <v>44650</v>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="1">
+        <v>44720</v>
       </c>
       <c r="B60" s="1">
         <v>45602</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
-        <v>44664</v>
+        <v>44734</v>
       </c>
       <c r="B61" s="1">
         <v>45630</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
-        <v>44678</v>
+        <v>44748</v>
       </c>
       <c r="B62" s="1">
         <v>45659</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
-        <v>44692</v>
+        <v>44762</v>
       </c>
       <c r="B63" s="1">
         <v>45700</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
-        <v>44706</v>
+        <v>44776</v>
       </c>
       <c r="B64" s="1">
         <v>45728</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
-        <v>44720</v>
+        <v>44790</v>
       </c>
       <c r="B65" s="1">
         <v>45756</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
-        <v>44734</v>
+        <v>44818</v>
       </c>
       <c r="B66" s="1">
         <v>45784</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
-        <v>44748</v>
+        <v>44832</v>
       </c>
       <c r="B67" s="1">
         <v>45812</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
-        <v>44762</v>
+        <v>44846</v>
       </c>
       <c r="B68" s="1">
         <v>45840</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
-        <v>44776</v>
+        <v>44860</v>
       </c>
       <c r="B69" s="1">
         <v>45882</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
-        <v>44790</v>
+        <v>44874</v>
       </c>
       <c r="B70" s="1">
         <v>45910</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A71" s="2">
-        <v>44804</v>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" s="1">
+        <v>44888</v>
       </c>
       <c r="B71" s="1">
         <v>45938</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
-        <v>44818</v>
+        <v>44902</v>
       </c>
       <c r="B72" s="1">
         <v>45966</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
-        <v>44832</v>
+        <v>44916</v>
       </c>
       <c r="B73" s="1">
         <v>45994</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
-        <v>44846</v>
+        <v>44930</v>
       </c>
       <c r="B74" s="1">
         <v>46036</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
-        <v>44860</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+        <v>44944</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
-        <v>44874</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+        <v>44958</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
-        <v>44888</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+        <v>44972</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
-        <v>44902</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+        <v>44986</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
-        <v>44916</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+        <v>45000</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
-        <v>44930</v>
-      </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+        <v>45028</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
-        <v>44944</v>
-      </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+        <v>45042</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
-        <v>44958</v>
-      </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
+        <v>45056</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
-        <v>44972</v>
-      </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+        <v>45070</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
-        <v>44986</v>
-      </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
-        <v>45000</v>
-      </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A86" s="2">
-        <v>45014</v>
-      </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
+        <v>45098</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" s="1">
+        <v>45112</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
-        <v>45028</v>
-      </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
+        <v>45126</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
-        <v>45042</v>
-      </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
+        <v>45140</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
-        <v>45056</v>
-      </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
+        <v>45154</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
-        <v>45070</v>
-      </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
+        <v>45182</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
-        <v>45084</v>
-      </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
+        <v>45196</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
-        <v>45098</v>
-      </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
+        <v>45210</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
-        <v>45112</v>
-      </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
+        <v>45224</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
-        <v>45126</v>
-      </c>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
+        <v>45238</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
-        <v>45140</v>
-      </c>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
+        <v>45252</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
-        <v>45154</v>
-      </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A97" s="2">
-        <v>45168</v>
-      </c>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
+        <v>45266</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" s="1">
+        <v>45280</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
-        <v>45182</v>
-      </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
+        <v>45294</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
-        <v>45196</v>
-      </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
+        <v>45308</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
-        <v>45210</v>
-      </c>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
+        <v>45336</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
-        <v>45224</v>
-      </c>
-    </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.3">
+        <v>45350</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
-        <v>45238</v>
-      </c>
-    </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.3">
+        <v>45364</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
-        <v>45252</v>
-      </c>
-    </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.3">
+        <v>45378</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
-        <v>45266</v>
-      </c>
-    </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.3">
+        <v>45392</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
-        <v>45280</v>
-      </c>
-    </row>
-    <row r="106" spans="1:1" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+        <v>45406</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
-        <v>45294</v>
-      </c>
-    </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.3">
+        <v>45420</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
-        <v>45308</v>
-      </c>
-    </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A108" s="2">
-        <v>45322</v>
-      </c>
-    </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.3">
+        <v>45434</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A108" s="1">
+        <v>45448</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
-        <v>45336</v>
-      </c>
-    </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.3">
+        <v>45461</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
-        <v>45350</v>
-      </c>
-    </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.3">
+        <v>45476</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
-        <v>45364</v>
-      </c>
-    </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.3">
+        <v>45490</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
-        <v>45378</v>
-      </c>
-    </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.3">
+        <v>45518</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
-        <v>45392</v>
-      </c>
-    </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.3">
+        <v>45532</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
-        <v>45406</v>
-      </c>
-    </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.3">
+        <v>45546</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
-        <v>45420</v>
-      </c>
-    </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.3">
+        <v>45560</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
-        <v>45434</v>
-      </c>
-    </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.3">
+        <v>45574</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
-        <v>45448</v>
-      </c>
-    </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.3">
+        <v>45588</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
-        <v>45461</v>
-      </c>
-    </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.3">
+        <v>45602</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
-        <v>45476</v>
-      </c>
-    </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.3">
+        <v>45616</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
-        <v>45490</v>
-      </c>
-    </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A121" s="2">
-        <v>45504</v>
-      </c>
-    </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.3">
+        <v>45630</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A121" s="1">
+        <v>45644</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
-        <v>45518</v>
-      </c>
-    </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.3">
+        <v>45659</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
-        <v>45532</v>
-      </c>
-    </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.3">
+        <v>45672</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
-        <v>45546</v>
-      </c>
-    </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.3">
+        <v>45700</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
-        <v>45560</v>
-      </c>
-    </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.3">
+        <v>45714</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
-        <v>45574</v>
-      </c>
-    </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.3">
+        <v>45728</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
-        <v>45588</v>
-      </c>
-    </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.3">
+        <v>45742</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
-        <v>45602</v>
-      </c>
-    </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.3">
+        <v>45756</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
-        <v>45616</v>
-      </c>
-    </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.3">
+        <v>45770</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
-        <v>45630</v>
-      </c>
-    </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.3">
+        <v>45784</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
-        <v>45644</v>
-      </c>
-    </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.3">
+        <v>45798</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
-        <v>45659</v>
-      </c>
-    </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.3">
+        <v>45812</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
-        <v>45672</v>
-      </c>
-    </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A134" s="2">
-        <v>45686</v>
-      </c>
-    </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.3">
+        <v>45826</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A134" s="1">
+        <v>45840</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
-        <v>45700</v>
-      </c>
-    </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.3">
+        <v>45854</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
-        <v>45714</v>
-      </c>
-    </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.3">
+        <v>45882</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
-        <v>45728</v>
-      </c>
-    </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.3">
+        <v>45896</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
-        <v>45742</v>
-      </c>
-    </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.3">
+        <v>45910</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
-        <v>45756</v>
-      </c>
-    </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.3">
+        <v>45924</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
-        <v>45770</v>
-      </c>
-    </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.3">
+        <v>45938</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
-        <v>45784</v>
-      </c>
-    </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.3">
+        <v>45952</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
-        <v>45798</v>
-      </c>
-    </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.3">
+        <v>45966</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
-        <v>45812</v>
-      </c>
-    </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.3">
+        <v>45980</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
-        <v>45826</v>
-      </c>
-    </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.3">
+        <v>45994</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
-        <v>45840</v>
-      </c>
-    </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.3">
+        <v>46008</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
-        <v>45854</v>
-      </c>
-    </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A147" s="2">
-        <v>45868</v>
-      </c>
-    </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A148" s="1">
-        <v>45882</v>
-      </c>
-    </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A149" s="1">
-        <v>45896</v>
-      </c>
-    </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A150" s="1">
-        <v>45910</v>
-      </c>
-    </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A151" s="1">
-        <v>45924</v>
-      </c>
-    </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A152" s="1">
-        <v>45938</v>
-      </c>
-    </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A153" s="1">
-        <v>45952</v>
-      </c>
-    </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A154" s="1">
-        <v>45966</v>
-      </c>
-    </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A155" s="1">
-        <v>45980</v>
-      </c>
-    </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A156" s="1">
-        <v>45994</v>
-      </c>
-    </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A157" s="1">
-        <v>46008</v>
-      </c>
-    </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A158" s="2">
-        <v>46021</v>
-      </c>
-    </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A159" s="1">
         <v>46036</v>
       </c>
     </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A160" s="1">
+    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A147" s="1">
         <v>46050</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:A147" xr:uid="{C55E9EE7-05DB-43E6-A4E4-0C41AA9632D9}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A147">
+      <sortCondition ref="A1:A147"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>